<commit_message>
update results with DE
</commit_message>
<xml_diff>
--- a/data/national_results/results_metadata.xlsx
+++ b/data/national_results/results_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/nelms_upenn_edu/Documents/Penn/Wharton/NLURI/wharton_gis_repo/data/national_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{5F763099-06C5-4F75-B7D7-421A877096D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC8AAB09-E025-45FD-9FC4-3B7365DF4175}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{5F763099-06C5-4F75-B7D7-421A877096D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B15F8492-68AA-47EA-8C38-91855C25812A}"/>
   <bookViews>
-    <workbookView xWindow="-26040" yWindow="2970" windowWidth="17280" windowHeight="8970" xr2:uid="{52A7EA2F-6563-4AD1-AD46-9B7589BAEBFD}"/>
+    <workbookView xWindow="-28920" yWindow="-1485" windowWidth="29040" windowHeight="15840" xr2:uid="{52A7EA2F-6563-4AD1-AD46-9B7589BAEBFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>